<commit_message>
update minutes iwith latest WG meetings
</commit_message>
<xml_diff>
--- a/data/wg_attendees.xlsx
+++ b/data/wg_attendees.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t xml:space="preserve">Winston Chang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margaret Wishart</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -161,13 +164,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -219,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,10 +232,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -252,128 +244,22 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,7 +434,7 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -559,8 +445,19 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -581,6 +478,7 @@
     <hyperlink ref="C15" r:id="rId14" display="https://appsilon.com"/>
     <hyperlink ref="C16" r:id="rId15" display="https://posit.co"/>
     <hyperlink ref="C17" r:id="rId16" display="https://posit.co"/>
+    <hyperlink ref="C18" r:id="rId17" display="https://www.bms.com/ "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>